<commit_message>
Completed data driven tests
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkumar\Desktop\pythonProject1\venv\Automation_for_git\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C567D2-68DD-4192-B25B-B2BC1A55CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67809455-6504-4D6E-9ACF-2C969BEAC5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8490CB00-EB6E-4701-9763-043E8625D8F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>secret_sauc</t>
   </si>
 </sst>
 </file>
@@ -472,7 +469,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -519,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -530,7 +527,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -541,10 +538,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -552,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added button functions logic
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkumar\Desktop\pythonProject1\venv\Automation_for_git\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67809455-6504-4D6E-9ACF-2C969BEAC5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBBD912-8BB7-41FE-B6E0-1D711BA31F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8490CB00-EB6E-4701-9763-043E8625D8F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -65,13 +65,10 @@
     <t>visual_user</t>
   </si>
   <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>secret_sauc</t>
   </si>
 </sst>
 </file>
@@ -469,7 +466,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,10 +491,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -505,10 +502,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -516,10 +513,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -527,10 +524,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -538,10 +535,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -549,10 +546,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>